<commit_message>
new classes for accept env
</commit_message>
<xml_diff>
--- a/src/test/resources/UnumTestdata.xlsx
+++ b/src/test/resources/UnumTestdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MariiaCherniak\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MariiaCherniak\Documents\GitHub\Unum\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624B21AE-02BD-4197-A06A-C2A4F31A6AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96CE985-FDB5-4E17-A1DF-9D7A8443C62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{87F6A5CC-70FA-4D56-9478-BCA61617E0BB}"/>
   </bookViews>
@@ -445,7 +445,7 @@
         <v>2</v>
       </c>
       <c r="D1">
-        <v>511307914</v>
+        <v>511377915</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>

</xml_diff>